<commit_message>
updated bewertungsbogen in coach meeting
</commit_message>
<xml_diff>
--- a/docs/Bewertungsbogen Projekte 5 und 6.xlsx
+++ b/docs/Bewertungsbogen Projekte 5 und 6.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aness\Dropbox\FHNW\004 Geteilte Ordner\IP5 - GrovePi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aness\github\IP5\GPIOSimulator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABACD518-2B6D-4AEE-BF3E-740EA85351B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB34F22C-1161-408D-9813-1100E16DD633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1744,6 +1744,48 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1772,9 +1814,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1788,45 +1827,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -5353,160 +5353,160 @@
       <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="157"/>
-      <c r="C8" s="157"/>
+      <c r="B8" s="170"/>
+      <c r="C8" s="170"/>
     </row>
     <row r="9" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="158"/>
-      <c r="C9" s="159"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="172"/>
     </row>
     <row r="10" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="30"/>
-      <c r="B10" s="160"/>
-      <c r="C10" s="161"/>
+      <c r="B10" s="173"/>
+      <c r="C10" s="174"/>
     </row>
     <row r="11" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="157"/>
-      <c r="C11" s="157"/>
+      <c r="B11" s="170"/>
+      <c r="C11" s="170"/>
     </row>
     <row r="12" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="157"/>
-      <c r="C12" s="157"/>
+      <c r="B12" s="170"/>
+      <c r="C12" s="170"/>
     </row>
     <row r="13" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="24"/>
       <c r="B13" s="25"/>
     </row>
     <row r="14" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="147" t="s">
+      <c r="A14" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="148"/>
-      <c r="C14" s="149"/>
+      <c r="B14" s="162"/>
+      <c r="C14" s="163"/>
     </row>
     <row r="15" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="150"/>
-      <c r="B15" s="151"/>
-      <c r="C15" s="152"/>
+      <c r="A15" s="164"/>
+      <c r="B15" s="165"/>
+      <c r="C15" s="166"/>
     </row>
     <row r="16" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="150"/>
-      <c r="B16" s="151"/>
-      <c r="C16" s="152"/>
+      <c r="A16" s="164"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="166"/>
     </row>
     <row r="17" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="150"/>
-      <c r="B17" s="151"/>
-      <c r="C17" s="152"/>
+      <c r="A17" s="164"/>
+      <c r="B17" s="165"/>
+      <c r="C17" s="166"/>
     </row>
     <row r="18" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="150"/>
-      <c r="B18" s="151"/>
-      <c r="C18" s="152"/>
+      <c r="A18" s="164"/>
+      <c r="B18" s="165"/>
+      <c r="C18" s="166"/>
     </row>
     <row r="19" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="150"/>
-      <c r="B19" s="151"/>
-      <c r="C19" s="152"/>
+      <c r="A19" s="164"/>
+      <c r="B19" s="165"/>
+      <c r="C19" s="166"/>
     </row>
     <row r="20" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="150"/>
-      <c r="B20" s="151"/>
-      <c r="C20" s="152"/>
+      <c r="A20" s="164"/>
+      <c r="B20" s="165"/>
+      <c r="C20" s="166"/>
     </row>
     <row r="21" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="150"/>
-      <c r="B21" s="151"/>
-      <c r="C21" s="152"/>
+      <c r="A21" s="164"/>
+      <c r="B21" s="165"/>
+      <c r="C21" s="166"/>
     </row>
     <row r="22" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="150"/>
-      <c r="B22" s="151"/>
-      <c r="C22" s="152"/>
+      <c r="A22" s="164"/>
+      <c r="B22" s="165"/>
+      <c r="C22" s="166"/>
     </row>
     <row r="23" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="150"/>
-      <c r="B23" s="151"/>
-      <c r="C23" s="152"/>
+      <c r="A23" s="164"/>
+      <c r="B23" s="165"/>
+      <c r="C23" s="166"/>
     </row>
     <row r="24" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="150"/>
-      <c r="B24" s="151"/>
-      <c r="C24" s="152"/>
+      <c r="A24" s="164"/>
+      <c r="B24" s="165"/>
+      <c r="C24" s="166"/>
     </row>
     <row r="25" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="150"/>
-      <c r="B25" s="151"/>
-      <c r="C25" s="152"/>
+      <c r="A25" s="164"/>
+      <c r="B25" s="165"/>
+      <c r="C25" s="166"/>
     </row>
     <row r="26" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="150"/>
-      <c r="B26" s="151"/>
-      <c r="C26" s="152"/>
+      <c r="A26" s="164"/>
+      <c r="B26" s="165"/>
+      <c r="C26" s="166"/>
     </row>
     <row r="27" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="150"/>
-      <c r="B27" s="151"/>
-      <c r="C27" s="152"/>
+      <c r="A27" s="164"/>
+      <c r="B27" s="165"/>
+      <c r="C27" s="166"/>
     </row>
     <row r="28" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="150"/>
-      <c r="B28" s="151"/>
-      <c r="C28" s="152"/>
+      <c r="A28" s="164"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="166"/>
     </row>
     <row r="29" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="150"/>
-      <c r="B29" s="151"/>
-      <c r="C29" s="152"/>
+      <c r="A29" s="164"/>
+      <c r="B29" s="165"/>
+      <c r="C29" s="166"/>
     </row>
     <row r="30" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="150"/>
-      <c r="B30" s="151"/>
-      <c r="C30" s="152"/>
+      <c r="A30" s="164"/>
+      <c r="B30" s="165"/>
+      <c r="C30" s="166"/>
     </row>
     <row r="31" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="150"/>
-      <c r="B31" s="151"/>
-      <c r="C31" s="152"/>
+      <c r="A31" s="164"/>
+      <c r="B31" s="165"/>
+      <c r="C31" s="166"/>
     </row>
     <row r="32" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="150"/>
-      <c r="B32" s="151"/>
-      <c r="C32" s="152"/>
+      <c r="A32" s="164"/>
+      <c r="B32" s="165"/>
+      <c r="C32" s="166"/>
     </row>
     <row r="33" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="150"/>
-      <c r="B33" s="151"/>
-      <c r="C33" s="152"/>
+      <c r="A33" s="164"/>
+      <c r="B33" s="165"/>
+      <c r="C33" s="166"/>
     </row>
     <row r="34" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="150"/>
-      <c r="B34" s="151"/>
-      <c r="C34" s="152"/>
+      <c r="A34" s="164"/>
+      <c r="B34" s="165"/>
+      <c r="C34" s="166"/>
     </row>
     <row r="35" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="153"/>
-      <c r="B35" s="154"/>
-      <c r="C35" s="155"/>
+      <c r="A35" s="167"/>
+      <c r="B35" s="168"/>
+      <c r="C35" s="169"/>
     </row>
     <row r="36" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="24"/>
       <c r="B36" s="25"/>
     </row>
     <row r="37" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="156" t="s">
+      <c r="A37" s="147" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="156"/>
+      <c r="B37" s="147"/>
       <c r="C37" s="31">
         <f>'2. Detailbewertung (Excel)'!C34</f>
         <v>0.2</v>
@@ -5517,30 +5517,30 @@
       <c r="B38" s="25"/>
     </row>
     <row r="39" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="156" t="s">
+      <c r="A39" s="147" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="156"/>
-      <c r="C39" s="156"/>
+      <c r="B39" s="147"/>
+      <c r="C39" s="147"/>
     </row>
     <row r="40" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="167" t="s">
+      <c r="A40" s="153" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="168"/>
-      <c r="C40" s="169"/>
+      <c r="B40" s="154"/>
+      <c r="C40" s="155"/>
     </row>
     <row r="41" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="170"/>
-      <c r="B41" s="171"/>
-      <c r="C41" s="172"/>
+      <c r="A41" s="156"/>
+      <c r="B41" s="157"/>
+      <c r="C41" s="158"/>
     </row>
     <row r="42" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="162" t="s">
+      <c r="A42" s="148" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="162"/>
-      <c r="C42" s="162"/>
+      <c r="B42" s="148"/>
+      <c r="C42" s="148"/>
     </row>
     <row r="43" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="24"/>
@@ -5554,48 +5554,54 @@
       <c r="A45" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="173">
+      <c r="B45" s="159">
         <f ca="1">TODAY()</f>
-        <v>43907</v>
-      </c>
-      <c r="C45" s="174"/>
+        <v>43909</v>
+      </c>
+      <c r="C45" s="160"/>
     </row>
     <row r="46" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="27"/>
-      <c r="B46" s="163"/>
-      <c r="C46" s="163"/>
+      <c r="B46" s="149"/>
+      <c r="C46" s="149"/>
     </row>
     <row r="47" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="27"/>
-      <c r="B47" s="163"/>
-      <c r="C47" s="163"/>
+      <c r="B47" s="149"/>
+      <c r="C47" s="149"/>
     </row>
     <row r="48" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B48" s="163"/>
-      <c r="C48" s="163"/>
+      <c r="B48" s="149"/>
+      <c r="C48" s="149"/>
     </row>
     <row r="49" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="28"/>
-      <c r="B49" s="163"/>
-      <c r="C49" s="163"/>
+      <c r="B49" s="149"/>
+      <c r="C49" s="149"/>
     </row>
     <row r="50" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="164"/>
-      <c r="C50" s="164"/>
+      <c r="B50" s="150"/>
+      <c r="C50" s="150"/>
     </row>
     <row r="51" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="29"/>
-      <c r="B51" s="165"/>
-      <c r="C51" s="166"/>
+      <c r="B51" s="151"/>
+      <c r="C51" s="152"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A14:C35"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B9:C10"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="B49:C49"/>
@@ -5606,12 +5612,6 @@
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B48:C48"/>
-    <mergeCell ref="A14:C35"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B9:C10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.68" right="0.19" top="0.25" bottom="0.97" header="0.96" footer="0.4921259845"/>
@@ -5625,7 +5625,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="74" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:D32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5929,7 +5931,7 @@
         <v>53</v>
       </c>
       <c r="C20" s="87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="62"/>
       <c r="E20" s="88"/>
@@ -5995,7 +5997,7 @@
         <v>60</v>
       </c>
       <c r="C24" s="61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="62"/>
       <c r="E24" s="118"/>
@@ -6014,7 +6016,7 @@
       </c>
       <c r="C25" s="84">
         <f>2-C24</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="62"/>
       <c r="E25" s="120"/>
@@ -6089,7 +6091,7 @@
         <v>7</v>
       </c>
       <c r="C30" s="182">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D30" s="183"/>
       <c r="E30" s="131"/>
@@ -6104,7 +6106,7 @@
         <v>8</v>
       </c>
       <c r="C31" s="182">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D31" s="183"/>
       <c r="E31" s="133"/>
@@ -6119,7 +6121,7 @@
         <v>49</v>
       </c>
       <c r="C32" s="184">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D32" s="185"/>
       <c r="E32" s="135"/>

</xml_diff>

<commit_message>
set motivation on bewertungsbogen
</commit_message>
<xml_diff>
--- a/docs/Bewertungsbogen Projekte 5 und 6.xlsx
+++ b/docs/Bewertungsbogen Projekte 5 und 6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aness\github\IP5\GPIOSimulator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB34F22C-1161-408D-9813-1100E16DD633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDBE63A-AF9B-4DE4-A130-387B8970FCD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1744,9 +1744,51 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1785,48 +1827,6 @@
     </xf>
     <xf numFmtId="14" fontId="23" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -5353,160 +5353,160 @@
       <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="170"/>
-      <c r="C8" s="170"/>
+      <c r="B8" s="157"/>
+      <c r="C8" s="157"/>
     </row>
     <row r="9" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="171"/>
-      <c r="C9" s="172"/>
+      <c r="B9" s="158"/>
+      <c r="C9" s="159"/>
     </row>
     <row r="10" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="30"/>
-      <c r="B10" s="173"/>
-      <c r="C10" s="174"/>
+      <c r="B10" s="160"/>
+      <c r="C10" s="161"/>
     </row>
     <row r="11" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="170"/>
-      <c r="C11" s="170"/>
+      <c r="B11" s="157"/>
+      <c r="C11" s="157"/>
     </row>
     <row r="12" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="170"/>
-      <c r="C12" s="170"/>
+      <c r="B12" s="157"/>
+      <c r="C12" s="157"/>
     </row>
     <row r="13" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="24"/>
       <c r="B13" s="25"/>
     </row>
     <row r="14" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="161" t="s">
+      <c r="A14" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="162"/>
-      <c r="C14" s="163"/>
+      <c r="B14" s="148"/>
+      <c r="C14" s="149"/>
     </row>
     <row r="15" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="164"/>
-      <c r="B15" s="165"/>
-      <c r="C15" s="166"/>
+      <c r="A15" s="150"/>
+      <c r="B15" s="151"/>
+      <c r="C15" s="152"/>
     </row>
     <row r="16" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="164"/>
-      <c r="B16" s="165"/>
-      <c r="C16" s="166"/>
+      <c r="A16" s="150"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="152"/>
     </row>
     <row r="17" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="164"/>
-      <c r="B17" s="165"/>
-      <c r="C17" s="166"/>
+      <c r="A17" s="150"/>
+      <c r="B17" s="151"/>
+      <c r="C17" s="152"/>
     </row>
     <row r="18" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="164"/>
-      <c r="B18" s="165"/>
-      <c r="C18" s="166"/>
+      <c r="A18" s="150"/>
+      <c r="B18" s="151"/>
+      <c r="C18" s="152"/>
     </row>
     <row r="19" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="164"/>
-      <c r="B19" s="165"/>
-      <c r="C19" s="166"/>
+      <c r="A19" s="150"/>
+      <c r="B19" s="151"/>
+      <c r="C19" s="152"/>
     </row>
     <row r="20" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="164"/>
-      <c r="B20" s="165"/>
-      <c r="C20" s="166"/>
+      <c r="A20" s="150"/>
+      <c r="B20" s="151"/>
+      <c r="C20" s="152"/>
     </row>
     <row r="21" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="164"/>
-      <c r="B21" s="165"/>
-      <c r="C21" s="166"/>
+      <c r="A21" s="150"/>
+      <c r="B21" s="151"/>
+      <c r="C21" s="152"/>
     </row>
     <row r="22" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="164"/>
-      <c r="B22" s="165"/>
-      <c r="C22" s="166"/>
+      <c r="A22" s="150"/>
+      <c r="B22" s="151"/>
+      <c r="C22" s="152"/>
     </row>
     <row r="23" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="164"/>
-      <c r="B23" s="165"/>
-      <c r="C23" s="166"/>
+      <c r="A23" s="150"/>
+      <c r="B23" s="151"/>
+      <c r="C23" s="152"/>
     </row>
     <row r="24" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="164"/>
-      <c r="B24" s="165"/>
-      <c r="C24" s="166"/>
+      <c r="A24" s="150"/>
+      <c r="B24" s="151"/>
+      <c r="C24" s="152"/>
     </row>
     <row r="25" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="164"/>
-      <c r="B25" s="165"/>
-      <c r="C25" s="166"/>
+      <c r="A25" s="150"/>
+      <c r="B25" s="151"/>
+      <c r="C25" s="152"/>
     </row>
     <row r="26" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="164"/>
-      <c r="B26" s="165"/>
-      <c r="C26" s="166"/>
+      <c r="A26" s="150"/>
+      <c r="B26" s="151"/>
+      <c r="C26" s="152"/>
     </row>
     <row r="27" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="164"/>
-      <c r="B27" s="165"/>
-      <c r="C27" s="166"/>
+      <c r="A27" s="150"/>
+      <c r="B27" s="151"/>
+      <c r="C27" s="152"/>
     </row>
     <row r="28" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="164"/>
-      <c r="B28" s="165"/>
-      <c r="C28" s="166"/>
+      <c r="A28" s="150"/>
+      <c r="B28" s="151"/>
+      <c r="C28" s="152"/>
     </row>
     <row r="29" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="164"/>
-      <c r="B29" s="165"/>
-      <c r="C29" s="166"/>
+      <c r="A29" s="150"/>
+      <c r="B29" s="151"/>
+      <c r="C29" s="152"/>
     </row>
     <row r="30" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="164"/>
-      <c r="B30" s="165"/>
-      <c r="C30" s="166"/>
+      <c r="A30" s="150"/>
+      <c r="B30" s="151"/>
+      <c r="C30" s="152"/>
     </row>
     <row r="31" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="164"/>
-      <c r="B31" s="165"/>
-      <c r="C31" s="166"/>
+      <c r="A31" s="150"/>
+      <c r="B31" s="151"/>
+      <c r="C31" s="152"/>
     </row>
     <row r="32" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="164"/>
-      <c r="B32" s="165"/>
-      <c r="C32" s="166"/>
+      <c r="A32" s="150"/>
+      <c r="B32" s="151"/>
+      <c r="C32" s="152"/>
     </row>
     <row r="33" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="164"/>
-      <c r="B33" s="165"/>
-      <c r="C33" s="166"/>
+      <c r="A33" s="150"/>
+      <c r="B33" s="151"/>
+      <c r="C33" s="152"/>
     </row>
     <row r="34" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="164"/>
-      <c r="B34" s="165"/>
-      <c r="C34" s="166"/>
+      <c r="A34" s="150"/>
+      <c r="B34" s="151"/>
+      <c r="C34" s="152"/>
     </row>
     <row r="35" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="167"/>
-      <c r="B35" s="168"/>
-      <c r="C35" s="169"/>
+      <c r="A35" s="153"/>
+      <c r="B35" s="154"/>
+      <c r="C35" s="155"/>
     </row>
     <row r="36" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="24"/>
       <c r="B36" s="25"/>
     </row>
     <row r="37" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="147" t="s">
+      <c r="A37" s="156" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="147"/>
+      <c r="B37" s="156"/>
       <c r="C37" s="31">
         <f>'2. Detailbewertung (Excel)'!C34</f>
         <v>0.2</v>
@@ -5517,30 +5517,30 @@
       <c r="B38" s="25"/>
     </row>
     <row r="39" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="147" t="s">
+      <c r="A39" s="156" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="147"/>
-      <c r="C39" s="147"/>
+      <c r="B39" s="156"/>
+      <c r="C39" s="156"/>
     </row>
     <row r="40" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="153" t="s">
+      <c r="A40" s="167" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="154"/>
-      <c r="C40" s="155"/>
+      <c r="B40" s="168"/>
+      <c r="C40" s="169"/>
     </row>
     <row r="41" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="156"/>
-      <c r="B41" s="157"/>
-      <c r="C41" s="158"/>
+      <c r="A41" s="170"/>
+      <c r="B41" s="171"/>
+      <c r="C41" s="172"/>
     </row>
     <row r="42" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="148" t="s">
+      <c r="A42" s="162" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="148"/>
-      <c r="C42" s="148"/>
+      <c r="B42" s="162"/>
+      <c r="C42" s="162"/>
     </row>
     <row r="43" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="24"/>
@@ -5554,54 +5554,48 @@
       <c r="A45" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="159">
+      <c r="B45" s="173">
         <f ca="1">TODAY()</f>
-        <v>43909</v>
-      </c>
-      <c r="C45" s="160"/>
+        <v>43914</v>
+      </c>
+      <c r="C45" s="174"/>
     </row>
     <row r="46" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="27"/>
-      <c r="B46" s="149"/>
-      <c r="C46" s="149"/>
+      <c r="B46" s="163"/>
+      <c r="C46" s="163"/>
     </row>
     <row r="47" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="27"/>
-      <c r="B47" s="149"/>
-      <c r="C47" s="149"/>
+      <c r="B47" s="163"/>
+      <c r="C47" s="163"/>
     </row>
     <row r="48" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B48" s="149"/>
-      <c r="C48" s="149"/>
+      <c r="B48" s="163"/>
+      <c r="C48" s="163"/>
     </row>
     <row r="49" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="28"/>
-      <c r="B49" s="149"/>
-      <c r="C49" s="149"/>
+      <c r="B49" s="163"/>
+      <c r="C49" s="163"/>
     </row>
     <row r="50" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="150"/>
-      <c r="C50" s="150"/>
+      <c r="B50" s="164"/>
+      <c r="C50" s="164"/>
     </row>
     <row r="51" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="29"/>
-      <c r="B51" s="151"/>
-      <c r="C51" s="152"/>
+      <c r="B51" s="165"/>
+      <c r="C51" s="166"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A14:C35"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B9:C10"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="B49:C49"/>
@@ -5612,6 +5606,12 @@
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B48:C48"/>
+    <mergeCell ref="A14:C35"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B9:C10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.68" right="0.19" top="0.25" bottom="0.97" header="0.96" footer="0.4921259845"/>
@@ -5625,8 +5625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="74" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:D32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="74" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -6033,7 +6033,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="84">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="62"/>
       <c r="E26" s="110"/>

</xml_diff>